<commit_message>
Using Lookup Functions (VLOOKUP) to Fill the Database Sheet
</commit_message>
<xml_diff>
--- a/Section 6/65. Discounting Cash Flows in Microsoft Excel/54.+FV+and+PV-Lecture.xlsx
+++ b/Section 6/65. Discounting Cash Flows in Microsoft Excel/54.+FV+and+PV-Lecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data_science\udemy_economics\Section 6\65. Discounting Cash Flows in Microsoft Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61E1421-44AC-4159-83E7-0E30FFE12E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8A9469-9080-4B32-B71F-781FBBFEFEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="270" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -613,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I20"/>
+  <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,6 +797,88 @@
         <f>SUM(C20:H20)</f>
         <v>-66.818585417041888</v>
       </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="3">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8">
+        <v>2</v>
+      </c>
+      <c r="F23" s="3">
+        <v>3</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="3">
+        <v>-500</v>
+      </c>
+      <c r="D24" s="3">
+        <v>30</v>
+      </c>
+      <c r="E24" s="8">
+        <v>120</v>
+      </c>
+      <c r="F24" s="3">
+        <v>200</v>
+      </c>
+      <c r="G24" s="3">
+        <v>120</v>
+      </c>
+      <c r="H24" s="3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+      <c r="C25" s="3">
+        <v>-500</v>
+      </c>
+      <c r="D25" s="3">
+        <f>D24/($C$4+1)^D23</f>
+        <v>27.27272727272727</v>
+      </c>
+      <c r="E25" s="3">
+        <f>E24/($C$4+1)^E23</f>
+        <v>99.173553719008254</v>
+      </c>
+      <c r="F25" s="3">
+        <f>F24/($C$4+1)^F23</f>
+        <v>150.2629601803155</v>
+      </c>
+      <c r="G25" s="3">
+        <f>G24/($C$4+1)^G23</f>
+        <v>81.96161464380846</v>
+      </c>
+      <c r="H25" s="3">
+        <f>H24/($C$4+1)^H23</f>
+        <v>74.510558767098601</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="16"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="2:9" ht="12" x14ac:dyDescent="0.2">
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>